<commit_message>
Add function selection and add function to give average as formula
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -115,8 +115,8 @@
   </sheetPr>
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:H16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -556,10 +556,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:H16"/>
+      <selection pane="topLeft" activeCell="M32" activeCellId="1" sqref="H1:H16 M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -592,6 +592,21 @@
       <c r="H1" s="0" t="n">
         <v>8</v>
       </c>
+      <c r="I1" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="J1" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="K1" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="L1" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="M1" s="0" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -618,6 +633,21 @@
       <c r="H2" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="I2" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -644,6 +674,21 @@
       <c r="H3" s="0" t="n">
         <v>24</v>
       </c>
+      <c r="I3" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -670,6 +715,21 @@
       <c r="H4" s="0" t="n">
         <v>32</v>
       </c>
+      <c r="I4" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>37</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -696,6 +756,21 @@
       <c r="H5" s="0" t="n">
         <v>40</v>
       </c>
+      <c r="I5" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>45</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -722,6 +797,21 @@
       <c r="H6" s="0" t="n">
         <v>48</v>
       </c>
+      <c r="I6" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>53</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -748,6 +838,21 @@
       <c r="H7" s="0" t="n">
         <v>56</v>
       </c>
+      <c r="I7" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>61</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -774,6 +879,21 @@
       <c r="H8" s="0" t="n">
         <v>64</v>
       </c>
+      <c r="I8" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>69</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -800,6 +920,21 @@
       <c r="H9" s="0" t="n">
         <v>72</v>
       </c>
+      <c r="I9" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>77</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -826,6 +961,21 @@
       <c r="H10" s="0" t="n">
         <v>80</v>
       </c>
+      <c r="I10" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>85</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -852,6 +1002,21 @@
       <c r="H11" s="0" t="n">
         <v>88</v>
       </c>
+      <c r="I11" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>93</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -878,6 +1043,21 @@
       <c r="H12" s="0" t="n">
         <v>96</v>
       </c>
+      <c r="I12" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>101</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -904,6 +1084,21 @@
       <c r="H13" s="0" t="n">
         <v>104</v>
       </c>
+      <c r="I13" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>106</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <v>109</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -930,6 +1125,21 @@
       <c r="H14" s="0" t="n">
         <v>112</v>
       </c>
+      <c r="I14" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>115</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <v>117</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -956,6 +1166,21 @@
       <c r="H15" s="0" t="n">
         <v>120</v>
       </c>
+      <c r="I15" s="0" t="n">
+        <v>121</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>122</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <v>125</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -981,6 +1206,513 @@
       </c>
       <c r="H16" s="0" t="n">
         <v>128</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>129</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>131</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <v>132</v>
+      </c>
+      <c r="M16" s="0" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>129</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>131</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>132</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>133</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>134</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>135</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>136</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>137</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>138</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>139</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <v>140</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>137</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>138</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>139</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>140</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>141</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>142</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>143</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>144</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>145</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>146</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="L18" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="M18" s="0" t="n">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>145</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>146</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>149</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>151</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>152</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>153</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>154</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>155</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <v>156</v>
+      </c>
+      <c r="M19" s="0" t="n">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>153</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>154</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>155</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>156</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>157</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>158</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>159</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>160</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>161</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>162</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <v>163</v>
+      </c>
+      <c r="L20" s="0" t="n">
+        <v>164</v>
+      </c>
+      <c r="M20" s="0" t="n">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>161</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>162</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>163</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>164</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>165</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>166</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>167</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>168</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>169</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <v>170</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <v>171</v>
+      </c>
+      <c r="L21" s="0" t="n">
+        <v>172</v>
+      </c>
+      <c r="M21" s="0" t="n">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>169</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>170</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>171</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>172</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>173</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>174</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>175</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>176</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>177</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>178</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <v>179</v>
+      </c>
+      <c r="L22" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="M22" s="0" t="n">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>177</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>178</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>179</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>181</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>182</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>183</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>184</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>185</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <v>186</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>187</v>
+      </c>
+      <c r="L23" s="0" t="n">
+        <v>188</v>
+      </c>
+      <c r="M23" s="0" t="n">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>185</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>186</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>187</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>188</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>189</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>190</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>191</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>192</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>193</v>
+      </c>
+      <c r="J24" s="0" t="n">
+        <v>194</v>
+      </c>
+      <c r="K24" s="0" t="n">
+        <v>195</v>
+      </c>
+      <c r="L24" s="0" t="n">
+        <v>196</v>
+      </c>
+      <c r="M24" s="0" t="n">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>193</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>194</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>195</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>196</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>197</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>198</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>199</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <v>201</v>
+      </c>
+      <c r="J25" s="0" t="n">
+        <v>202</v>
+      </c>
+      <c r="K25" s="0" t="n">
+        <v>203</v>
+      </c>
+      <c r="L25" s="0" t="n">
+        <v>204</v>
+      </c>
+      <c r="M25" s="0" t="n">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>201</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>202</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>203</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>204</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>205</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>206</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>207</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>208</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <v>209</v>
+      </c>
+      <c r="J26" s="0" t="n">
+        <v>210</v>
+      </c>
+      <c r="K26" s="0" t="n">
+        <v>211</v>
+      </c>
+      <c r="L26" s="0" t="n">
+        <v>212</v>
+      </c>
+      <c r="M26" s="0" t="n">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>209</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>210</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>211</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>212</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>213</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>214</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>215</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>216</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>217</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <v>218</v>
+      </c>
+      <c r="K27" s="0" t="n">
+        <v>219</v>
+      </c>
+      <c r="L27" s="0" t="n">
+        <v>220</v>
+      </c>
+      <c r="M27" s="0" t="n">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>217</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>218</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>219</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>220</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>221</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>222</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>223</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <v>224</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <v>225</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <v>226</v>
+      </c>
+      <c r="K28" s="0" t="n">
+        <v>227</v>
+      </c>
+      <c r="L28" s="0" t="n">
+        <v>228</v>
+      </c>
+      <c r="M28" s="0" t="n">
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -999,10 +1731,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:H16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="H1:H16 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1035,6 +1767,39 @@
       <c r="H1" s="0" t="n">
         <v>8</v>
       </c>
+      <c r="I1" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="J1" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="K1" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="L1" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="M1" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="N1" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="O1" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="P1" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="R1" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="S1" s="0" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -1061,6 +1826,39 @@
       <c r="H2" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="I2" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q2" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="R2" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="S2" s="0" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -1087,6 +1885,39 @@
       <c r="H3" s="0" t="n">
         <v>24</v>
       </c>
+      <c r="I3" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="P3" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="R3" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="S3" s="0" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -1113,6 +1944,39 @@
       <c r="H4" s="0" t="n">
         <v>32</v>
       </c>
+      <c r="I4" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="S4" s="0" t="n">
+        <v>43</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -1139,6 +2003,39 @@
       <c r="H5" s="0" t="n">
         <v>40</v>
       </c>
+      <c r="I5" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <v>51</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -1165,6 +2062,39 @@
       <c r="H6" s="0" t="n">
         <v>48</v>
       </c>
+      <c r="I6" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="P6" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="S6" s="0" t="n">
+        <v>59</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -1191,6 +2121,39 @@
       <c r="H7" s="0" t="n">
         <v>56</v>
       </c>
+      <c r="I7" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="P7" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="Q7" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="R7" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="S7" s="0" t="n">
+        <v>67</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -1217,6 +2180,39 @@
       <c r="H8" s="0" t="n">
         <v>64</v>
       </c>
+      <c r="I8" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="P8" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="Q8" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="R8" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="S8" s="0" t="n">
+        <v>75</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -1243,6 +2239,39 @@
       <c r="H9" s="0" t="n">
         <v>72</v>
       </c>
+      <c r="I9" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="P9" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="R9" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="S9" s="0" t="n">
+        <v>83</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -1269,6 +2298,39 @@
       <c r="H10" s="0" t="n">
         <v>80</v>
       </c>
+      <c r="I10" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="P10" s="0" t="n">
+        <v>88</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="R10" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="S10" s="0" t="n">
+        <v>91</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -1295,6 +2357,39 @@
       <c r="H11" s="0" t="n">
         <v>88</v>
       </c>
+      <c r="I11" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="P11" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="Q11" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="R11" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="S11" s="0" t="n">
+        <v>99</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -1321,6 +2416,39 @@
       <c r="H12" s="0" t="n">
         <v>96</v>
       </c>
+      <c r="I12" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="P12" s="0" t="n">
+        <v>104</v>
+      </c>
+      <c r="Q12" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="R12" s="0" t="n">
+        <v>106</v>
+      </c>
+      <c r="S12" s="0" t="n">
+        <v>107</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -1347,6 +2475,39 @@
       <c r="H13" s="0" t="n">
         <v>104</v>
       </c>
+      <c r="I13" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>106</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="P13" s="0" t="n">
+        <v>112</v>
+      </c>
+      <c r="Q13" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="R13" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="S13" s="0" t="n">
+        <v>115</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -1373,6 +2534,39 @@
       <c r="H14" s="0" t="n">
         <v>112</v>
       </c>
+      <c r="I14" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>115</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <v>118</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <v>119</v>
+      </c>
+      <c r="P14" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <v>121</v>
+      </c>
+      <c r="R14" s="0" t="n">
+        <v>122</v>
+      </c>
+      <c r="S14" s="0" t="n">
+        <v>123</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -1399,6 +2593,39 @@
       <c r="H15" s="0" t="n">
         <v>120</v>
       </c>
+      <c r="I15" s="0" t="n">
+        <v>121</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>122</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <v>125</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <v>126</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <v>127</v>
+      </c>
+      <c r="P15" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="Q15" s="0" t="n">
+        <v>129</v>
+      </c>
+      <c r="R15" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="S15" s="0" t="n">
+        <v>131</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -1424,6 +2651,39 @@
       </c>
       <c r="H16" s="0" t="n">
         <v>128</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>129</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>131</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <v>132</v>
+      </c>
+      <c r="M16" s="0" t="n">
+        <v>133</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <v>134</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <v>135</v>
+      </c>
+      <c r="P16" s="0" t="n">
+        <v>136</v>
+      </c>
+      <c r="Q16" s="0" t="n">
+        <v>137</v>
+      </c>
+      <c r="R16" s="0" t="n">
+        <v>138</v>
+      </c>
+      <c r="S16" s="0" t="n">
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>